<commit_message>
Update Verified.xlsx with new parts.
</commit_message>
<xml_diff>
--- a/design/MagellanSolidworks/Visio/Verified.xlsx
+++ b/design/MagellanSolidworks/Visio/Verified.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09A06C6-1A00-4567-811F-D9EED81BA5D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9251AEE-78F8-4B9F-B9A0-DDF06EC07688}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>Component Name</t>
   </si>
@@ -101,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,12 +111,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF4519"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,11 +133,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,16 +425,16 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" activeCellId="1" sqref="B14 B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -463,7 +456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -474,7 +467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -485,7 +478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -496,7 +489,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -507,26 +500,29 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="b">
+      <c r="B8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -537,18 +533,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="b">
-        <v>0</v>
+      <c r="B10" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -559,40 +555,40 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="b">
+      <c r="B12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="b">
-        <v>0</v>
+      <c r="B13" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="3" t="b">
+      <c r="B14" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -603,18 +599,18 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="b">
-        <v>0</v>
+      <c r="B16" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
WIP commit. Base plates filled out, still need to do crossbar and top plate.
</commit_message>
<xml_diff>
--- a/design/MagellanSolidworks/Visio/Verified.xlsx
+++ b/design/MagellanSolidworks/Visio/Verified.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9251AEE-78F8-4B9F-B9A0-DDF06EC07688}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BCF2F1-3442-40E3-8C0B-E7DF4C59A033}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="23">
   <si>
     <t>Component Name</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Mango</t>
+  </si>
+  <si>
+    <t>Circuit Breaker</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +483,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="b">
         <v>0</v>
@@ -491,29 +494,29 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2" t="b">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>1</v>
@@ -524,51 +527,51 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="b">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="b">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="b">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="B11" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="b">
         <v>1</v>
@@ -579,7 +582,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="2" t="b">
         <v>1</v>
@@ -590,34 +593,45 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="b">
+      <c r="B18" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>